<commit_message>
Finished all, need only logs
</commit_message>
<xml_diff>
--- a/BitcoinPriceTracker/Data/Config.xlsx
+++ b/BitcoinPriceTracker/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrei Gabor\Desktop\UNI\3rd YEAR\RPA\RPAProject\BitcoinPriceTracker\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF6E14A-7079-49DF-B19A-7798503AC653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32A670E-4F7C-4303-98E2-36D52C2985DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48195" yWindow="2535" windowWidth="17910" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30945" yWindow="2040" windowWidth="17910" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -31,49 +31,67 @@
     <t>pricesExcelPath</t>
   </si>
   <si>
+    <t>binanceURL</t>
+  </si>
+  <si>
+    <t>https://www.binance.com/en/trade/BTC_BUSD</t>
+  </si>
+  <si>
+    <t>kucoinURL</t>
+  </si>
+  <si>
+    <t>https://trade.kucoin.com/BTC-USDT</t>
+  </si>
+  <si>
+    <t>coinbaseURL</t>
+  </si>
+  <si>
+    <t>https://www.coinbase.com/price/bitcoin</t>
+  </si>
+  <si>
+    <t>cmcURL</t>
+  </si>
+  <si>
+    <t>https://coinmarketcap.com/currencies/bitcoin/</t>
+  </si>
+  <si>
+    <t>coingeckoURL</t>
+  </si>
+  <si>
+    <t>https://www.coingecko.com/ro/coins/bitcoin</t>
+  </si>
+  <si>
+    <t>cursURL</t>
+  </si>
+  <si>
+    <t>https://www.cursbnr.ro/</t>
+  </si>
+  <si>
+    <t>emailsPath</t>
+  </si>
+  <si>
+    <t>C:\Users\Andrei Gabor\Desktop\UNI\3rd YEAR\RPA\RPAProject\BitcoinPriceTracker\Data\emails.txt</t>
+  </si>
+  <si>
+    <t>emailSubject</t>
+  </si>
+  <si>
+    <t>emailBodySuccess</t>
+  </si>
+  <si>
+    <t>emailBodyFailure</t>
+  </si>
+  <si>
+    <t>Bitcoin Prices</t>
+  </si>
+  <si>
+    <t>Dear user, an error occurred.</t>
+  </si>
+  <si>
+    <t>Dear user, here is the attachment from the run made at {0}.</t>
+  </si>
+  <si>
     <t>C:\Users\Andrei Gabor\Desktop\UNI\3rd YEAR\RPA\RPAProject\BitcoinPriceTracker\Data\prices.xlsx</t>
-  </si>
-  <si>
-    <t>binanceURL</t>
-  </si>
-  <si>
-    <t>https://www.binance.com/en/trade/BTC_BUSD</t>
-  </si>
-  <si>
-    <t>kucoinURL</t>
-  </si>
-  <si>
-    <t>https://trade.kucoin.com/BTC-USDT</t>
-  </si>
-  <si>
-    <t>coinbaseURL</t>
-  </si>
-  <si>
-    <t>https://www.coinbase.com/price/bitcoin</t>
-  </si>
-  <si>
-    <t>cmcURL</t>
-  </si>
-  <si>
-    <t>https://coinmarketcap.com/currencies/bitcoin/</t>
-  </si>
-  <si>
-    <t>coingeckoURL</t>
-  </si>
-  <si>
-    <t>https://www.coingecko.com/ro/coins/bitcoin</t>
-  </si>
-  <si>
-    <t>cursURL</t>
-  </si>
-  <si>
-    <t>https://www.cursbnr.ro/</t>
-  </si>
-  <si>
-    <t>emailsPath</t>
-  </si>
-  <si>
-    <t>C:\Users\Andrei Gabor\Desktop\UNI\3rd YEAR\RPA\RPAProject\BitcoinPriceTracker\Data\emails.txt</t>
   </si>
 </sst>
 </file>
@@ -458,7 +476,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -506,70 +524,91 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.4">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>7</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
         <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Changed SendEmail without ForEach
</commit_message>
<xml_diff>
--- a/BitcoinPriceTracker/Data/Config.xlsx
+++ b/BitcoinPriceTracker/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrei Gabor\Desktop\UNI\3rd YEAR\RPA\RPAProject\BitcoinPriceTracker\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32A670E-4F7C-4303-98E2-36D52C2985DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7AE508-3088-4C60-B8ED-386B94CB5F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30945" yWindow="2040" windowWidth="17910" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>C:\Users\Andrei Gabor\Desktop\UNI\3rd YEAR\RPA\RPAProject\BitcoinPriceTracker\Data\prices.xlsx</t>
+  </si>
+  <si>
+    <t>attachment</t>
   </si>
 </sst>
 </file>
@@ -476,7 +479,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -609,7 +612,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>